<commit_message>
Implemented Deals Test - nonDDT
</commit_message>
<xml_diff>
--- a/FreeCRMTestAutomation/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
+++ b/FreeCRMTestAutomation/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
@@ -7,16 +7,16 @@
     <workbookView xWindow="360" yWindow="135" windowWidth="16215" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="contacts" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="deals" sheetId="2" r:id="rId1"/>
+    <sheet name="contacts" sheetId="1" r:id="rId2"/>
+    <sheet name="tasks" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="74">
   <si>
     <t>title</t>
   </si>
@@ -64,6 +64,180 @@
   </si>
   <si>
     <t>Ebay</t>
+  </si>
+  <si>
+    <t>primaryContact</t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Option No 1</t>
+  </si>
+  <si>
+    <t>Option No 2</t>
+  </si>
+  <si>
+    <t>Option No 3</t>
+  </si>
+  <si>
+    <t>Option No 4</t>
+  </si>
+  <si>
+    <t>Option No 5</t>
+  </si>
+  <si>
+    <t>Option No 6</t>
+  </si>
+  <si>
+    <t>Option No 7</t>
+  </si>
+  <si>
+    <t>Option No 8</t>
+  </si>
+  <si>
+    <t>Option No 9</t>
+  </si>
+  <si>
+    <t>Option No 10</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Tesla</t>
+  </si>
+  <si>
+    <t>Yahoo</t>
+  </si>
+  <si>
+    <t>Netflix</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>Spotify</t>
+  </si>
+  <si>
+    <t>Sony</t>
+  </si>
+  <si>
+    <t>Nintendo</t>
+  </si>
+  <si>
+    <t>Mike Michaels</t>
+  </si>
+  <si>
+    <t>John Johnnies</t>
+  </si>
+  <si>
+    <t>Elsa Pato</t>
+  </si>
+  <si>
+    <t>Aqui Meando</t>
+  </si>
+  <si>
+    <t>Elsa Patazo</t>
+  </si>
+  <si>
+    <t>Lucila Manguera</t>
+  </si>
+  <si>
+    <t>Eldo Larcito</t>
+  </si>
+  <si>
+    <t>Amy Garchota</t>
+  </si>
+  <si>
+    <t>Susana Oria</t>
+  </si>
+  <si>
+    <t>Satoshi Nakamura</t>
+  </si>
+  <si>
+    <t>alc</t>
+  </si>
+  <si>
+    <t>pra</t>
+  </si>
+  <si>
+    <t>rei</t>
+  </si>
+  <si>
+    <t>fez</t>
+  </si>
+  <si>
+    <t>aqp</t>
+  </si>
+  <si>
+    <t>peh</t>
+  </si>
+  <si>
+    <t>ric</t>
+  </si>
+  <si>
+    <t>kae</t>
+  </si>
+  <si>
+    <t>ova</t>
+  </si>
+  <si>
+    <t>pae</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>Lad</t>
+  </si>
+  <si>
+    <t>pants</t>
+  </si>
+  <si>
+    <t>ravin</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Old</t>
+  </si>
+  <si>
+    <t>Opportunity</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Existing Customer</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>Referral</t>
+  </si>
+  <si>
+    <t>Word of Mouth</t>
   </si>
 </sst>
 </file>
@@ -402,10 +576,276 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -467,18 +907,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>